<commit_message>
atualização da tabela para os meus casos de uso
</commit_message>
<xml_diff>
--- a/Gerência de Projetos/Divisão dos casos de uso - Temporário.xlsx
+++ b/Gerência de Projetos/Divisão dos casos de uso - Temporário.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>UC01</t>
   </si>
@@ -432,7 +432,7 @@
   <dimension ref="B3:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,7 +521,12 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1">
+        <v>40282</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">

</xml_diff>